<commit_message>
CRUD users and orders, access patterns
</commit_message>
<xml_diff>
--- a/files/db-modelling.xlsx
+++ b/files/db-modelling.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
   <si>
     <t>pk</t>
   </si>
@@ -36,12 +36,6 @@
     <t>XP_SingleTableDdb</t>
   </si>
   <si>
-    <t>USER#adrianosastre</t>
-  </si>
-  <si>
-    <t>USER#isabella</t>
-  </si>
-  <si>
     <t>PROFILE#adrianosastre</t>
   </si>
   <si>
@@ -157,6 +151,15 @@
   </si>
   <si>
     <t>GSI (inverter sk/pk), pk = sk</t>
+  </si>
+  <si>
+    <t>USER#</t>
+  </si>
+  <si>
+    <t>1. CRUD usuários</t>
+  </si>
+  <si>
+    <t>2. CRUD pedidos</t>
   </si>
 </sst>
 </file>
@@ -214,10 +217,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
@@ -503,7 +507,7 @@
   <dimension ref="B1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,220 +532,230 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4">
         <v>20210626</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="F6">
         <v>20210626</v>
       </c>
       <c r="G6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
         <v>33</v>
-      </c>
-      <c r="E14" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C29" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -750,6 +764,7 @@
     <hyperlink ref="E6" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Documentation added, fullName added to orders items on dynamoDB table
</commit_message>
<xml_diff>
--- a/files/db-modelling.xlsx
+++ b/files/db-modelling.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="50">
   <si>
     <t>pk</t>
   </si>
@@ -48,9 +48,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>createdAt</t>
-  </si>
-  <si>
     <t>addresses</t>
   </si>
   <si>
@@ -78,36 +75,9 @@
     <t>ORDER#2</t>
   </si>
   <si>
-    <t>2. Buscar pedidos de um usuário</t>
-  </si>
-  <si>
-    <t>1. Buscar perfil de um usuário</t>
-  </si>
-  <si>
-    <t>3. Buscar itens de um pedido</t>
-  </si>
-  <si>
-    <t>4. Buscar pedidos de um usuário por status</t>
-  </si>
-  <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>items</t>
   </si>
   <si>
-    <t>pk = X, sk BEGINS WITH PROFILE#</t>
-  </si>
-  <si>
-    <t>pk = X, sk BEGINS WITH ORDER#</t>
-  </si>
-  <si>
-    <t>GSI (inverter sk/pk), pk = X</t>
-  </si>
-  <si>
-    <t>LSI (status)</t>
-  </si>
-  <si>
     <t>ORDER#3</t>
   </si>
   <si>
@@ -147,26 +117,201 @@
     <t>ORDER#5</t>
   </si>
   <si>
-    <t>5. Buscar todos os usuários</t>
-  </si>
-  <si>
-    <t>GSI (inverter sk/pk), pk = sk</t>
-  </si>
-  <si>
     <t>USER#</t>
   </si>
   <si>
-    <t>1. CRUD usuários</t>
-  </si>
-  <si>
-    <t>2. CRUD pedidos</t>
+    <t>PADRÕES DE ACESSO:</t>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Listar perfil (detalhes) de um usuário</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Adicionar usuário</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Editar usuário</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Deletar usuário</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Listar todos os pedidos de um usuário *</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Listar pedidos de um usuário por status *</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Adicionar pedido de um usuário *</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Editar pedido de um usuário *</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Deletar pedido de um usuário</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>// Buscar itens de um pedido de um usuário *</t>
+    </r>
+  </si>
+  <si>
+    <t>orderStatus</t>
+  </si>
+  <si>
+    <r>
+      <t>       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>USUÁRIOS:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>PEDIDOS:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Listar todos os usuários</t>
+    </r>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>{"home":"one"}</t>
+  </si>
+  <si>
+    <t>{"home":"two"}</t>
+  </si>
+  <si>
+    <t>{"home":"three"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -188,6 +333,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -217,11 +373,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
@@ -504,25 +661,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:G29"/>
+  <dimension ref="B1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39" customWidth="1"/>
-    <col min="3" max="7" width="37.28515625" customWidth="1"/>
-    <col min="8" max="10" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="7" width="22.28515625" customWidth="1"/>
+    <col min="8" max="8" width="25.85546875" customWidth="1"/>
+    <col min="9" max="9" width="32.140625" customWidth="1"/>
+    <col min="10" max="10" width="30.140625" customWidth="1"/>
+    <col min="11" max="11" width="37.28515625" customWidth="1"/>
+    <col min="12" max="14" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -530,9 +691,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -546,27 +707,21 @@
       <c r="F3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="2" t="s">
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
+      <c r="E4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="F4">
-        <v>20210626</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -580,183 +735,267 @@
       <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="2" t="s">
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6">
-        <v>20210626</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="G8" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="G12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>37</v>
-      </c>
-      <c r="C15" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>17</v>
-      </c>
-      <c r="C25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C29" t="s">
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
         <v>41</v>
       </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="4"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>